<commit_message>
Update CC incidence calib data description
</commit_message>
<xml_diff>
--- a/Config/Validation_target-Globocan_registry_CC_inc.xlsx
+++ b/Config/Validation_target-Globocan_registry_CC_inc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" tabRatio="620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" tabRatio="620"/>
   </bookViews>
   <sheets>
     <sheet name="CCinc" sheetId="8" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>AGE GROUP</t>
   </si>
@@ -147,13 +147,13 @@
     <t>Globocan 2012 South African Republic CC incidence data</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: not quite sure how age-specific rates were accessed </t>
-  </si>
-  <si>
     <t>Minimum of PROMEC bounds, SA Registry bounds, &amp; Globocan data</t>
   </si>
   <si>
     <t>Maximum of PROMEC bounds, SA Registry bounds, &amp; Globocan data</t>
+  </si>
+  <si>
+    <t>Monisha emailed a connection to get age-specific rates</t>
   </si>
 </sst>
 </file>
@@ -454,6 +454,1258 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CC Incidence</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Rates</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>PROMEC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>CCinc!$A$10:$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>15-</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20-</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25-</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30-</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35-</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40-</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45-</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50-</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55-</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60-</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65-</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70-</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75-</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CCinc!$D$10:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0029989669110642</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.353499040899274</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.128220300055279</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.240942178375178</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33.977883486748624</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.408391435290234</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50.419303390440909</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>104.12838417248561</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>96.68526333668683</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57.296221464973918</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70.020402496589526</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7F73-4DAA-B0F8-5D19E1A1550F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>South Africa Registry</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>CCinc!$A$10:$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>15-</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20-</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25-</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30-</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35-</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40-</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45-</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50-</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55-</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60-</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65-</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70-</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75-</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CCinc!$M$10:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55.57</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>66.33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63.17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70.98</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>73.930000000000007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>83.11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92.88</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>72.760000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7F73-4DAA-B0F8-5D19E1A1550F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Globocan</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>CCinc!$A$10:$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>15-</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20-</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25-</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30-</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35-</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40-</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45-</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50-</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55-</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60-</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65-</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70-</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75-</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CCinc!$C$28:$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.646467153656904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.848389035625793</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.193737900145855</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.40682333812245</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>82.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7F73-4DAA-B0F8-5D19E1A1550F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1858454560"/>
+        <c:axId val="1858452064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1858454560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1858452064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1858452064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1858454560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10583</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>14817</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>613833</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>535517</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -743,28 +1995,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" customWidth="1"/>
-    <col min="14" max="14" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>40</v>
       </c>
@@ -778,7 +2030,7 @@
       <c r="N1" s="29"/>
       <c r="O1" s="29"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
@@ -796,7 +2048,7 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>20</v>
       </c>
@@ -808,7 +2060,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>29</v>
       </c>
@@ -817,7 +2069,7 @@
       </c>
       <c r="C4" s="23"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>17</v>
       </c>
@@ -828,7 +2080,7 @@
         <v>17100199</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>30</v>
       </c>
@@ -837,13 +2089,13 @@
       </c>
       <c r="C6" s="23"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:18" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:19" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -883,10 +2135,12 @@
       <c r="P9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Q9" s="1"/>
+      <c r="Q9" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>2</v>
       </c>
@@ -929,9 +2183,19 @@
       <c r="P10" s="21">
         <v>0</v>
       </c>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:18" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q10" s="1">
+        <f>(M10/100000)*L10</f>
+        <v>0.3515103</v>
+      </c>
+      <c r="R10">
+        <f>(SUM(Q10:Q14)/SUM(L10:L14))*100000</f>
+        <v>7.3139872994685806</v>
+      </c>
+      <c r="S10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>3</v>
       </c>
@@ -974,9 +2238,12 @@
       <c r="P11" s="10">
         <v>0</v>
       </c>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q11" s="1">
+        <f t="shared" ref="Q11:Q22" si="3">(M11/100000)*L11</f>
+        <v>0.57826579999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
@@ -995,11 +2262,11 @@
         <v>3.3534990408992741E-5</v>
       </c>
       <c r="F12" s="10">
-        <f t="shared" ref="F12:F22" si="3">(E12-1.96*SQRT((1/B12)*(E12)*(1-E12)))*100000</f>
+        <f t="shared" ref="F12:F22" si="4">(E12-1.96*SQRT((1/B12)*(E12)*(1-E12)))*100000</f>
         <v>0.41407681625798648</v>
       </c>
       <c r="G12" s="10">
-        <f t="shared" ref="G12:G22" si="4">(E12+1.96*SQRT((1/B12)*(E12)*(1-E12)))*100000</f>
+        <f t="shared" ref="G12:G22" si="5">(E12+1.96*SQRT((1/B12)*(E12)*(1-E12)))*100000</f>
         <v>6.2929212655405617</v>
       </c>
       <c r="K12" s="9" t="s">
@@ -1016,16 +2283,19 @@
         <v>4.9800000000000004E-5</v>
       </c>
       <c r="O12" s="10">
-        <f t="shared" ref="O12:O22" si="5">(N12-1.96*SQRT((1/L12)*(N12)*(1-N12)))*100000</f>
+        <f t="shared" ref="O12:O22" si="6">(N12-1.96*SQRT((1/L12)*(N12)*(1-N12)))*100000</f>
         <v>1.3980128824107521</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" ref="P12:P22" si="6">(N12+1.96*SQRT((1/L12)*(N12)*(1-N12)))*100000</f>
+        <f t="shared" ref="P12:P22" si="7">(N12+1.96*SQRT((1/L12)*(N12)*(1-N12)))*100000</f>
         <v>8.5619871175892488</v>
       </c>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q12" s="1">
+        <f t="shared" si="3"/>
+        <v>7.4250804000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>5</v>
       </c>
@@ -1044,11 +2314,11 @@
         <v>1.7128220300055279E-4</v>
       </c>
       <c r="F13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.9714055740770302</v>
       </c>
       <c r="G13" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24.285035026033526</v>
       </c>
       <c r="K13" s="9" t="s">
@@ -1065,16 +2335,19 @@
         <v>1.7339999999999999E-4</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10.139084063629639</v>
       </c>
       <c r="P13" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24.540915936370357</v>
       </c>
-      <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:18" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q13" s="1">
+        <f t="shared" si="3"/>
+        <v>22.272016199999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
@@ -1093,11 +2366,11 @@
         <v>2.0240942178375177E-4</v>
       </c>
       <c r="F14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.606787476749254</v>
       </c>
       <c r="G14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27.875096880001099</v>
       </c>
       <c r="K14" s="9" t="s">
@@ -1114,16 +2387,19 @@
         <v>3.1920000000000001E-4</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22.333685601446405</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>41.506314398553599</v>
       </c>
-      <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:18" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q14" s="1">
+        <f t="shared" si="3"/>
+        <v>42.579045600000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
@@ -1142,11 +2418,11 @@
         <v>3.3977883486748623E-4</v>
       </c>
       <c r="F15" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.999518530321875</v>
       </c>
       <c r="G15" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>42.956248443175369</v>
       </c>
       <c r="K15" s="9" t="s">
@@ -1163,16 +2439,19 @@
         <v>5.5570000000000001E-4</v>
       </c>
       <c r="O15" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44.089193848521049</v>
       </c>
       <c r="P15" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>67.050806151478952</v>
       </c>
-      <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:18" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1">
+        <f t="shared" si="3"/>
+        <v>89.951159000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
@@ -1191,11 +2470,11 @@
         <v>5.9408391435290234E-4</v>
       </c>
       <c r="F16" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45.689829935406607</v>
       </c>
       <c r="G16" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.126952935173861</v>
       </c>
       <c r="K16" s="9" t="s">
@@ -1212,16 +2491,19 @@
         <v>6.6330000000000002E-4</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>51.834785816502986</v>
       </c>
       <c r="P16" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80.82521418349701</v>
       </c>
-      <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q16" s="1">
+        <f t="shared" si="3"/>
+        <v>80.388643500000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>9</v>
       </c>
@@ -1240,11 +2522,11 @@
         <v>5.0419303390440912E-4</v>
       </c>
       <c r="F17" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.305457838445989</v>
       </c>
       <c r="G17" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>64.53314894243583</v>
       </c>
       <c r="K17" s="9" t="s">
@@ -1261,16 +2543,19 @@
         <v>6.3170000000000001E-4</v>
       </c>
       <c r="O17" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>47.372997930331501</v>
       </c>
       <c r="P17" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.96700206966851</v>
       </c>
-      <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1">
+        <f t="shared" si="3"/>
+        <v>61.391764500000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>10</v>
       </c>
@@ -1289,11 +2574,11 @@
         <v>1.0412838417248561E-3</v>
       </c>
       <c r="F18" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>79.391527399392302</v>
       </c>
       <c r="G18" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>128.8652409455789</v>
       </c>
       <c r="K18" s="9" t="s">
@@ -1310,16 +2595,19 @@
         <v>7.0980000000000001E-4</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50.553216247482311</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>91.406783752517683</v>
       </c>
-      <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q18" s="1">
+        <f t="shared" si="3"/>
+        <v>46.352779200000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
@@ -1338,11 +2626,11 @@
         <v>8.7000000000000001E-4</v>
       </c>
       <c r="F19" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68.726291309753236</v>
       </c>
       <c r="G19" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>105.27370869024676</v>
       </c>
       <c r="K19" s="9" t="s">
@@ -1359,16 +2647,19 @@
         <v>7.3930000000000003E-4</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>57.083649659777301</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>90.776350340222706</v>
       </c>
-      <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q19" s="1">
+        <f t="shared" si="3"/>
+        <v>73.930000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>12</v>
       </c>
@@ -1387,11 +2678,11 @@
         <v>9.6685263336686832E-4</v>
       </c>
       <c r="F20" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74.666625664626039</v>
       </c>
       <c r="G20" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>118.70390100874762</v>
       </c>
       <c r="K20" s="9" t="s">
@@ -1408,16 +2699,19 @@
         <v>8.3109999999999998E-4</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62.694197828849489</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>103.5258021711505</v>
       </c>
-      <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" ht="13" x14ac:dyDescent="0.25">
+      <c r="Q20" s="1">
+        <f t="shared" si="3"/>
+        <v>63.609900699999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>13</v>
       </c>
@@ -1436,11 +2730,11 @@
         <v>5.7296221464973917E-4</v>
       </c>
       <c r="F21" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>42.425906304331015</v>
       </c>
       <c r="G21" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.166536625616814</v>
       </c>
       <c r="K21" s="9" t="s">
@@ -1457,16 +2751,19 @@
         <v>9.2879999999999992E-4</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>73.950420879998575</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>111.8095791200014</v>
       </c>
-      <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q21" s="1">
+        <f t="shared" si="3"/>
+        <v>92.399810399999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>14</v>
       </c>
@@ -1485,11 +2782,11 @@
         <v>7.002040249658953E-4</v>
       </c>
       <c r="F22" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>52.00621922508671</v>
       </c>
       <c r="G22" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>88.034585768092356</v>
       </c>
       <c r="K22" s="12" t="s">
@@ -1506,16 +2803,19 @@
         <v>7.2760000000000001E-4</v>
       </c>
       <c r="O22" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>54.39704088054814</v>
       </c>
       <c r="P22" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>91.122959119451863</v>
       </c>
-      <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="Q22" s="1">
+        <f t="shared" si="3"/>
+        <v>60.2692908</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B23" s="15" t="s">
         <v>31</v>
       </c>
@@ -1538,7 +2838,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
         <v>41</v>
       </c>
@@ -1552,7 +2852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="24"/>
       <c r="B28" s="1"/>
       <c r="C28" s="26">
@@ -1568,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="24"/>
       <c r="B29" s="1"/>
       <c r="C29" s="26">
@@ -1576,15 +2876,15 @@
       </c>
       <c r="D29" s="1"/>
       <c r="F29" s="28">
-        <f t="shared" ref="F29:F40" si="7">MIN(F11,G11,O11,P11,C29)</f>
+        <f t="shared" ref="F29:F40" si="8">MIN(F11,G11,O11,P11,C29)</f>
         <v>0</v>
       </c>
       <c r="G29" s="28">
-        <f t="shared" ref="G29:G40" si="8">MAX(F11,G11,O11,P11,C29)</f>
+        <f t="shared" ref="G29:G40" si="9">MAX(F11,G11,O11,P11,C29)</f>
         <v>2.646467153656904</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="24"/>
       <c r="B30" s="1"/>
       <c r="C30" s="26">
@@ -1592,15 +2892,15 @@
       </c>
       <c r="D30" s="1"/>
       <c r="F30" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.41407681625798648</v>
       </c>
       <c r="G30" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.848389035625793</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="24"/>
       <c r="B31" s="1"/>
       <c r="C31" s="26">
@@ -1608,15 +2908,15 @@
       </c>
       <c r="D31" s="1"/>
       <c r="F31" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.9714055740770302</v>
       </c>
       <c r="G31" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>45.193737900145855</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="25">
         <v>21.9</v>
       </c>
@@ -1630,15 +2930,15 @@
         <v>23</v>
       </c>
       <c r="F32" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12.606787476749254</v>
       </c>
       <c r="G32" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>53.40682333812245</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="25">
         <v>63.4</v>
       </c>
@@ -1648,15 +2948,15 @@
       </c>
       <c r="D33" s="1"/>
       <c r="F33" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24.999518530321875</v>
       </c>
       <c r="G33" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>67.050806151478952</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="25">
         <v>68.3</v>
       </c>
@@ -1666,15 +2966,15 @@
       </c>
       <c r="D34" s="1"/>
       <c r="F34" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>45.689829935406607</v>
       </c>
       <c r="G34" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>80.82521418349701</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="25">
         <v>70.7</v>
       </c>
@@ -1684,15 +2984,15 @@
       </c>
       <c r="D35" s="1"/>
       <c r="F35" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>36.305457838445989</v>
       </c>
       <c r="G35" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>78.96700206966851</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="25">
         <v>73</v>
       </c>
@@ -1702,15 +3002,15 @@
       </c>
       <c r="D36" s="1"/>
       <c r="F36" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>50.553216247482311</v>
       </c>
       <c r="G36" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>128.8652409455789</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="25">
         <v>77.400000000000006</v>
       </c>
@@ -1722,15 +3022,15 @@
         <v>1</v>
       </c>
       <c r="F37" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>57.083649659777301</v>
       </c>
       <c r="G37" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>105.27370869024676</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="25">
         <v>82.7</v>
       </c>
@@ -1740,15 +3040,15 @@
       </c>
       <c r="D38" s="1"/>
       <c r="F38" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>62.694197828849489</v>
       </c>
       <c r="G38" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>118.70390100874762</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="25">
         <v>88.6</v>
       </c>
@@ -1758,15 +3058,15 @@
       </c>
       <c r="D39" s="1"/>
       <c r="F39" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>42.425906304331015</v>
       </c>
       <c r="G39" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>111.8095791200014</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="25">
         <v>95.2</v>
       </c>
@@ -1776,23 +3076,23 @@
       </c>
       <c r="D40" s="1"/>
       <c r="F40" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>52.00621922508671</v>
       </c>
       <c r="G40" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>95.2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="G41" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1804,5 +3104,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Globocan 2018 CC inc by age data to Excel doc
</commit_message>
<xml_diff>
--- a/Config/Validation_target-Globocan_registry_CC_inc.xlsx
+++ b/Config/Validation_target-Globocan_registry_CC_inc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" tabRatio="620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="620"/>
   </bookViews>
   <sheets>
     <sheet name="CCinc" sheetId="8" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>AGE GROUP</t>
   </si>
@@ -154,6 +154,32 @@
   </si>
   <si>
     <t>Monisha emailed a connection to get age-specific rates</t>
+  </si>
+  <si>
+    <t>Globocan 2018 South African Republic CC incidence data</t>
+  </si>
+  <si>
+    <t>Age Group</t>
+  </si>
+  <si>
+    <t>Raw cases</t>
+  </si>
+  <si>
+    <t>Crude Rate</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Data from Minttu at Harvard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Globocan incidence - https://gco.iarc.fr/today/
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numbers:  https://www.hpvcentre.net/statistics/reports/ZAF.pdf?t=1562271302543 (figure 7)
+</t>
   </si>
 </sst>
 </file>
@@ -163,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -184,6 +210,12 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -349,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -429,6 +461,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -437,6 +472,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -805,7 +861,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Globocan</c:v>
+            <c:v>Globocan 2012</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -930,6 +986,88 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7F73-4DAA-B0F8-5D19E1A1550F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Globocan 2018</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>CCinc!$C$46:$C$57</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3.9070527772503256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.718592555074853</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.815396540774046</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.753954608683522</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.181262777416052</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.090519192952186</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95.443618498222065</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96.099524161750054</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94.851577973825016</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>97.48752644071628</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>101.98823806664386</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110.42515650113373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-44DB-4EFB-930C-24EB72CA99DB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1995,10 +2133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P51" sqref="P51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2017,18 +2155,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="K1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="K1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
@@ -2041,12 +2179,12 @@
       <c r="K2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
@@ -2839,11 +2977,11 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="1"/>
       <c r="F27" s="27" t="s">
         <v>26</v>
@@ -2938,7 +3076,7 @@
         <v>53.40682333812245</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="25">
         <v>63.4</v>
       </c>
@@ -2956,7 +3094,7 @@
         <v>67.050806151478952</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="25">
         <v>68.3</v>
       </c>
@@ -2974,7 +3112,7 @@
         <v>80.82521418349701</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="25">
         <v>70.7</v>
       </c>
@@ -2992,7 +3130,7 @@
         <v>78.96700206966851</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="25">
         <v>73</v>
       </c>
@@ -3010,7 +3148,7 @@
         <v>128.8652409455789</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="25">
         <v>77.400000000000006</v>
       </c>
@@ -3030,7 +3168,7 @@
         <v>105.27370869024676</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="25">
         <v>82.7</v>
       </c>
@@ -3048,7 +3186,7 @@
         <v>118.70390100874762</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="25">
         <v>88.6</v>
       </c>
@@ -3066,7 +3204,7 @@
         <v>111.8095791200014</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="25">
         <v>95.2</v>
       </c>
@@ -3084,7 +3222,7 @@
         <v>95.2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
         <v>44</v>
       </c>
@@ -3095,12 +3233,224 @@
         <v>43</v>
       </c>
     </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="38">
+        <v>100</v>
+      </c>
+      <c r="C46" s="39">
+        <v>3.9070527772503256</v>
+      </c>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="33"/>
+      <c r="L46" s="33"/>
+      <c r="M46" s="33"/>
+      <c r="N46" s="33"/>
+      <c r="O46" s="33"/>
+      <c r="P46" s="33"/>
+      <c r="Q46" s="33"/>
+    </row>
+    <row r="47" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="38">
+        <v>503</v>
+      </c>
+      <c r="C47" s="39">
+        <v>19.718592555074853</v>
+      </c>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="34"/>
+      <c r="L47" s="34"/>
+      <c r="M47" s="34"/>
+      <c r="N47" s="34"/>
+      <c r="O47" s="34"/>
+      <c r="P47" s="34"/>
+      <c r="Q47" s="34"/>
+    </row>
+    <row r="48" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="38">
+        <v>913</v>
+      </c>
+      <c r="C48" s="39">
+        <v>35.815396540774046</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="38">
+        <v>1310</v>
+      </c>
+      <c r="C49" s="39">
+        <v>53.753954608683522</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="38">
+        <v>1501</v>
+      </c>
+      <c r="C50" s="39">
+        <v>71.181262777416052</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="38">
+        <v>1511</v>
+      </c>
+      <c r="C51" s="39">
+        <v>85.090519192952186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="38">
+        <v>1498</v>
+      </c>
+      <c r="C52" s="39">
+        <v>95.443618498222065</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="38">
+        <v>1320</v>
+      </c>
+      <c r="C53" s="39">
+        <v>96.099524161750054</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="38">
+        <v>1123</v>
+      </c>
+      <c r="C54" s="39">
+        <v>94.851577973825016</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="38">
+        <v>966</v>
+      </c>
+      <c r="C55" s="39">
+        <v>97.48752644071628</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="38">
+        <v>766</v>
+      </c>
+      <c r="C56" s="39">
+        <v>101.98823806664386</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="38">
+        <v>562</v>
+      </c>
+      <c r="C57" s="39">
+        <v>110.42515650113373</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="38">
+        <v>902</v>
+      </c>
+      <c r="C58" s="39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+    </row>
+    <row r="61" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A44:C44"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A59:C59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>